<commit_message>
finished tallying cacao count
</commit_message>
<xml_diff>
--- a/data/data-entry/CRCA_CBC_2023_Sensoria_data_entry.xlsx
+++ b/data/data-entry/CRCA_CBC_2023_Sensoria_data_entry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/An/github/ACG-CBC-data/data/data-entry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8743CBA-E90C-8A4F-8CB3-77432B0295CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA13B93B-FD34-4145-9FA7-BCF24AF2E75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="1080" windowWidth="28040" windowHeight="17440" xr2:uid="{7483F0A7-F4DD-ED49-9576-23FBD2807B8C}"/>
+    <workbookView xWindow="2200" yWindow="1080" windowWidth="28040" windowHeight="17440" xr2:uid="{7483F0A7-F4DD-ED49-9576-23FBD2807B8C}"/>
   </bookViews>
   <sheets>
     <sheet name="datos" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="470">
   <si>
     <t>localidad</t>
   </si>
@@ -1425,6 +1425,27 @@
   </si>
   <si>
     <t>Merlin</t>
+  </si>
+  <si>
+    <t>intersection Ruta 921 and Calle San Luis</t>
+  </si>
+  <si>
+    <t>Bella Vista, Dos Ríos</t>
+  </si>
+  <si>
+    <t>camino entre Dos Ríos and El Gavilán</t>
+  </si>
+  <si>
+    <t>Sensoria entrance</t>
+  </si>
+  <si>
+    <t>road between Quebrada Azufrada and Río Negro</t>
+  </si>
+  <si>
+    <t>road between Río Negro and Buenos Aires</t>
+  </si>
+  <si>
+    <t>El Gavilán</t>
   </si>
 </sst>
 </file>
@@ -1457,18 +1478,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1510,9 +1525,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1895,14 +1910,14 @@
   <dimension ref="A1:F222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C208" sqref="C208"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
     <col min="3" max="3" width="38.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
   </cols>
@@ -1911,7 +1926,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1928,7 +1943,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="6">
+      <c r="A2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B2" s="5">
         <v>0.3</v>
       </c>
       <c r="C2" t="s">
@@ -1945,7 +1963,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="6">
+      <c r="A3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B3" s="5">
         <v>0.3</v>
       </c>
       <c r="C3" t="s">
@@ -1959,7 +1980,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="6">
+      <c r="A4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4" s="5">
         <v>0.3</v>
       </c>
       <c r="C4" t="s">
@@ -1973,7 +1997,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="6">
+      <c r="A5" t="s">
+        <v>463</v>
+      </c>
+      <c r="B5" s="5">
         <v>0.3</v>
       </c>
       <c r="C5" t="s">
@@ -1990,7 +2017,7 @@
       <c r="A6" t="s">
         <v>450</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.30416666666666664</v>
       </c>
       <c r="C6" t="s">
@@ -2007,7 +2034,7 @@
       <c r="A7" t="s">
         <v>450</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.30416666666666664</v>
       </c>
       <c r="C7" t="s">
@@ -2024,7 +2051,7 @@
       <c r="A8" t="s">
         <v>450</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>0.30555555555555552</v>
       </c>
       <c r="C8" t="s">
@@ -2044,7 +2071,7 @@
       <c r="A9" t="s">
         <v>450</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.30555555555555552</v>
       </c>
       <c r="C9" t="s">
@@ -2061,7 +2088,7 @@
       <c r="A10" t="s">
         <v>450</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0.30555555555555552</v>
       </c>
       <c r="C10" t="s">
@@ -2081,7 +2108,7 @@
       <c r="A11" t="s">
         <v>450</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>0.30694444444444441</v>
       </c>
       <c r="C11" t="s">
@@ -2098,7 +2125,7 @@
       <c r="A12" t="s">
         <v>450</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>0.30833333333333335</v>
       </c>
       <c r="C12" t="s">
@@ -2115,7 +2142,7 @@
       <c r="A13" t="s">
         <v>450</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>0.30833333333333335</v>
       </c>
       <c r="C13" t="s">
@@ -2132,7 +2159,7 @@
       <c r="A14" t="s">
         <v>450</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>0.30833333333333335</v>
       </c>
       <c r="C14" t="s">
@@ -2152,7 +2179,7 @@
       <c r="A15" t="s">
         <v>450</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>0.30972222222222223</v>
       </c>
       <c r="C15" t="s">
@@ -2169,7 +2196,7 @@
       <c r="A16" t="s">
         <v>450</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>0.31111111111111112</v>
       </c>
       <c r="C16" t="s">
@@ -2186,7 +2213,7 @@
       <c r="A17" t="s">
         <v>450</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>0.31180555555555556</v>
       </c>
       <c r="C17" t="s">
@@ -2203,7 +2230,7 @@
       <c r="A18" t="s">
         <v>450</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>0.3125</v>
       </c>
       <c r="C18" t="s">
@@ -2220,7 +2247,7 @@
       <c r="A19" t="s">
         <v>450</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>0.3125</v>
       </c>
       <c r="C19" t="s">
@@ -2237,7 +2264,7 @@
       <c r="A20" t="s">
         <v>450</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>0.31319444444444444</v>
       </c>
       <c r="C20" t="s">
@@ -2254,7 +2281,7 @@
       <c r="A21" t="s">
         <v>450</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>0.31319444444444444</v>
       </c>
       <c r="C21" t="s">
@@ -2271,7 +2298,7 @@
       <c r="A22" t="s">
         <v>450</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>0.31388888888888888</v>
       </c>
       <c r="C22" t="s">
@@ -2288,7 +2315,7 @@
       <c r="A23" t="s">
         <v>450</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>0.31527777777777777</v>
       </c>
       <c r="C23" t="s">
@@ -2305,7 +2332,7 @@
       <c r="A24" t="s">
         <v>450</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>0.31597222222222221</v>
       </c>
       <c r="C24" t="s">
@@ -2322,7 +2349,7 @@
       <c r="A25" t="s">
         <v>450</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>0.31736111111111115</v>
       </c>
       <c r="C25" t="s">
@@ -2339,7 +2366,7 @@
       <c r="A26" t="s">
         <v>450</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>0.31805555555555554</v>
       </c>
       <c r="C26" t="s">
@@ -2356,7 +2383,7 @@
       <c r="A27" t="s">
         <v>450</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>0.32291666666666669</v>
       </c>
       <c r="C27" t="s">
@@ -2376,7 +2403,7 @@
       <c r="A28" t="s">
         <v>450</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>0.32361111111111113</v>
       </c>
       <c r="C28" t="s">
@@ -2393,7 +2420,7 @@
       <c r="A29" t="s">
         <v>450</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>0.32430555555555557</v>
       </c>
       <c r="C29" t="s">
@@ -2407,7 +2434,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="6">
+      <c r="A30" t="s">
+        <v>464</v>
+      </c>
+      <c r="B30" s="5">
         <v>0.32916666666666666</v>
       </c>
       <c r="C30" t="s">
@@ -2424,7 +2454,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B31" s="6">
+      <c r="A31" t="s">
+        <v>464</v>
+      </c>
+      <c r="B31" s="5">
         <v>0.33194444444444443</v>
       </c>
       <c r="C31" t="s">
@@ -2438,7 +2471,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="6">
+      <c r="A32" t="s">
+        <v>464</v>
+      </c>
+      <c r="B32" s="5">
         <v>0.33194444444444443</v>
       </c>
       <c r="C32" t="s">
@@ -2451,8 +2487,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>464</v>
+      </c>
+      <c r="B33" s="5">
         <v>0.33194444444444443</v>
       </c>
       <c r="C33" t="s">
@@ -2465,8 +2504,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>464</v>
+      </c>
+      <c r="B34" s="5">
         <v>0.33263888888888887</v>
       </c>
       <c r="C34" t="s">
@@ -2479,8 +2521,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>464</v>
+      </c>
+      <c r="B35" s="5">
         <v>0.33263888888888887</v>
       </c>
       <c r="C35" t="s">
@@ -2493,8 +2538,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>464</v>
+      </c>
+      <c r="B36" s="5">
         <v>0.33263888888888887</v>
       </c>
       <c r="C36" t="s">
@@ -2507,8 +2555,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B37" s="6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>464</v>
+      </c>
+      <c r="B37" s="5">
         <v>0.3347222222222222</v>
       </c>
       <c r="C37" t="s">
@@ -2521,8 +2572,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" s="6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>464</v>
+      </c>
+      <c r="B38" s="5">
         <v>0.3347222222222222</v>
       </c>
       <c r="C38" t="s">
@@ -2535,8 +2589,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>464</v>
+      </c>
+      <c r="B39" s="5">
         <v>0.33749999999999997</v>
       </c>
       <c r="C39" t="s">
@@ -2549,8 +2606,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>464</v>
+      </c>
+      <c r="B40" s="5">
         <v>0.33749999999999997</v>
       </c>
       <c r="C40" t="s">
@@ -2563,8 +2623,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>464</v>
+      </c>
+      <c r="B41" s="5">
         <v>0.33819444444444446</v>
       </c>
       <c r="C41" t="s">
@@ -2577,8 +2640,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>464</v>
+      </c>
+      <c r="B42" s="5">
         <v>0.33888888888888885</v>
       </c>
       <c r="C42" t="s">
@@ -2591,8 +2657,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>464</v>
+      </c>
+      <c r="B43" s="5">
         <v>0.33958333333333335</v>
       </c>
       <c r="C43" t="s">
@@ -2608,8 +2677,11 @@
         <v>455</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>465</v>
+      </c>
+      <c r="B44" s="5">
         <v>0.34236111111111112</v>
       </c>
       <c r="C44" t="s">
@@ -2622,8 +2694,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>465</v>
+      </c>
+      <c r="B45" s="5">
         <v>0.34236111111111112</v>
       </c>
       <c r="C45" t="s">
@@ -2636,8 +2711,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B46" s="6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>465</v>
+      </c>
+      <c r="B46" s="5">
         <v>0.34236111111111112</v>
       </c>
       <c r="C46" t="s">
@@ -2650,8 +2728,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B47" s="6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>465</v>
+      </c>
+      <c r="B47" s="5">
         <v>0.34375</v>
       </c>
       <c r="C47" t="s">
@@ -2664,8 +2745,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>465</v>
+      </c>
+      <c r="B48" s="5">
         <v>0.3444444444444445</v>
       </c>
       <c r="C48" t="s">
@@ -2678,8 +2762,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B49" s="6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>465</v>
+      </c>
+      <c r="B49" s="5">
         <v>0.3444444444444445</v>
       </c>
       <c r="C49" t="s">
@@ -2692,8 +2779,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B50" s="6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>465</v>
+      </c>
+      <c r="B50" s="5">
         <v>0.3444444444444445</v>
       </c>
       <c r="C50" t="s">
@@ -2706,8 +2796,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>465</v>
+      </c>
+      <c r="B51" s="5">
         <v>0.34652777777777777</v>
       </c>
       <c r="C51" t="s">
@@ -2720,8 +2813,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B52" s="6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>465</v>
+      </c>
+      <c r="B52" s="5">
         <v>0.35069444444444442</v>
       </c>
       <c r="C52" t="s">
@@ -2734,8 +2830,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B53" s="6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>465</v>
+      </c>
+      <c r="B53" s="5">
         <v>0.3527777777777778</v>
       </c>
       <c r="C53" t="s">
@@ -2748,8 +2847,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B54" s="6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>465</v>
+      </c>
+      <c r="B54" s="5">
         <v>0.35347222222222219</v>
       </c>
       <c r="C54" t="s">
@@ -2762,8 +2864,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B55" s="6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>466</v>
+      </c>
+      <c r="B55" s="5">
         <v>0.35972222222222222</v>
       </c>
       <c r="C55" t="s">
@@ -2776,8 +2881,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B56" s="6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>466</v>
+      </c>
+      <c r="B56" s="5">
         <v>0.36458333333333331</v>
       </c>
       <c r="C56" t="s">
@@ -2790,8 +2898,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B57" s="6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>466</v>
+      </c>
+      <c r="B57" s="5">
         <v>0.36458333333333331</v>
       </c>
       <c r="C57" t="s">
@@ -2804,8 +2915,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B58" s="6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>466</v>
+      </c>
+      <c r="B58" s="5">
         <v>0.36874999999999997</v>
       </c>
       <c r="C58" t="s">
@@ -2818,8 +2932,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B59" s="6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>466</v>
+      </c>
+      <c r="B59" s="5">
         <v>0.37708333333333338</v>
       </c>
       <c r="C59" t="s">
@@ -2835,8 +2952,11 @@
         <v>454</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B60" s="6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>466</v>
+      </c>
+      <c r="B60" s="5">
         <v>0.37708333333333338</v>
       </c>
       <c r="C60" t="s">
@@ -2849,8 +2969,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B61" s="6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>466</v>
+      </c>
+      <c r="B61" s="5">
         <v>0.37986111111111115</v>
       </c>
       <c r="C61" t="s">
@@ -2863,8 +2986,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B62" s="6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>466</v>
+      </c>
+      <c r="B62" s="5">
         <v>0.37986111111111115</v>
       </c>
       <c r="C62" t="s">
@@ -2877,8 +3003,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B63" s="6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>466</v>
+      </c>
+      <c r="B63" s="5">
         <v>0.3840277777777778</v>
       </c>
       <c r="C63" t="s">
@@ -2891,8 +3020,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B64" s="6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>466</v>
+      </c>
+      <c r="B64" s="5">
         <v>0.38611111111111113</v>
       </c>
       <c r="C64" t="s">
@@ -2908,8 +3040,11 @@
         <v>453</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B65" s="6">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>466</v>
+      </c>
+      <c r="B65" s="5">
         <v>0.39097222222222222</v>
       </c>
       <c r="C65" t="s">
@@ -2922,8 +3057,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B66" s="6">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>466</v>
+      </c>
+      <c r="B66" s="5">
         <v>0.39652777777777781</v>
       </c>
       <c r="C66" t="s">
@@ -2936,8 +3074,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B67" s="6">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>466</v>
+      </c>
+      <c r="B67" s="5">
         <v>0.39652777777777781</v>
       </c>
       <c r="C67" t="s">
@@ -2950,8 +3091,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B68" s="6">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>466</v>
+      </c>
+      <c r="B68" s="5">
         <v>0.40277777777777773</v>
       </c>
       <c r="C68" t="s">
@@ -2964,8 +3108,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B69" s="6">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>466</v>
+      </c>
+      <c r="B69" s="5">
         <v>0.4145833333333333</v>
       </c>
       <c r="C69" t="s">
@@ -2978,8 +3125,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B70" s="6">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>466</v>
+      </c>
+      <c r="B70" s="5">
         <v>0.41666666666666669</v>
       </c>
       <c r="C70" t="s">
@@ -2992,8 +3142,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B71" s="6">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>466</v>
+      </c>
+      <c r="B71" s="5">
         <v>0.41666666666666669</v>
       </c>
       <c r="C71" t="s">
@@ -3006,8 +3159,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B72" s="6">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>466</v>
+      </c>
+      <c r="B72" s="5">
         <v>0.42291666666666666</v>
       </c>
       <c r="C72" t="s">
@@ -3020,8 +3176,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B73" s="6">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>466</v>
+      </c>
+      <c r="B73" s="5">
         <v>0.4284722222222222</v>
       </c>
       <c r="C73" t="s">
@@ -3034,8 +3193,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B74" s="6">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>466</v>
+      </c>
+      <c r="B74" s="5">
         <v>0.43124999999999997</v>
       </c>
       <c r="C74" t="s">
@@ -3048,8 +3210,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B75" s="6">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>466</v>
+      </c>
+      <c r="B75" s="5">
         <v>0.43124999999999997</v>
       </c>
       <c r="C75" t="s">
@@ -3062,8 +3227,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B76" s="6">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>466</v>
+      </c>
+      <c r="B76" s="5">
         <v>0.43333333333333335</v>
       </c>
       <c r="C76" t="s">
@@ -3076,8 +3244,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B77" s="6">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>466</v>
+      </c>
+      <c r="B77" s="5">
         <v>0.4381944444444445</v>
       </c>
       <c r="C77" t="s">
@@ -3090,8 +3261,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B78" s="6">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>466</v>
+      </c>
+      <c r="B78" s="5">
         <v>0.44027777777777777</v>
       </c>
       <c r="C78" t="s">
@@ -3104,8 +3278,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B79" s="6">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>466</v>
+      </c>
+      <c r="B79" s="5">
         <v>0.44305555555555554</v>
       </c>
       <c r="C79" t="s">
@@ -3118,8 +3295,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B80" s="6">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>466</v>
+      </c>
+      <c r="B80" s="5">
         <v>0.4465277777777778</v>
       </c>
       <c r="C80" t="s">
@@ -3133,6 +3313,9 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>466</v>
+      </c>
       <c r="C81" t="s">
         <v>364</v>
       </c>
@@ -3147,7 +3330,7 @@
       <c r="A82" t="s">
         <v>457</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="5">
         <v>0.44861111111111113</v>
       </c>
       <c r="C82" t="s">
@@ -3164,7 +3347,10 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B83" s="6">
+      <c r="A83" t="s">
+        <v>457</v>
+      </c>
+      <c r="B83" s="5">
         <v>0.44861111111111113</v>
       </c>
       <c r="C83" t="s">
@@ -3178,7 +3364,10 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B84" s="6">
+      <c r="A84" t="s">
+        <v>457</v>
+      </c>
+      <c r="B84" s="5">
         <v>0.44930555555555557</v>
       </c>
       <c r="C84" t="s">
@@ -3192,7 +3381,10 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B85" s="6">
+      <c r="A85" t="s">
+        <v>457</v>
+      </c>
+      <c r="B85" s="5">
         <v>0.45347222222222222</v>
       </c>
       <c r="C85" t="s">
@@ -3206,7 +3398,10 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B86" s="6">
+      <c r="A86" t="s">
+        <v>457</v>
+      </c>
+      <c r="B86" s="5">
         <v>0.45347222222222222</v>
       </c>
       <c r="C86" t="s">
@@ -3220,7 +3415,10 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B87" s="6">
+      <c r="A87" t="s">
+        <v>457</v>
+      </c>
+      <c r="B87" s="5">
         <v>0.45347222222222222</v>
       </c>
       <c r="C87" t="s">
@@ -3234,7 +3432,10 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B88" s="6">
+      <c r="A88" t="s">
+        <v>457</v>
+      </c>
+      <c r="B88" s="5">
         <v>0.46249999999999997</v>
       </c>
       <c r="C88" t="s">
@@ -3248,7 +3449,10 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B89" s="6">
+      <c r="A89" t="s">
+        <v>457</v>
+      </c>
+      <c r="B89" s="5">
         <v>0.46249999999999997</v>
       </c>
       <c r="C89" t="s">
@@ -3262,6 +3466,9 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>457</v>
+      </c>
       <c r="C90" t="s">
         <v>216</v>
       </c>
@@ -3273,6 +3480,9 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>457</v>
+      </c>
       <c r="C91" t="s">
         <v>353</v>
       </c>
@@ -3284,6 +3494,9 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>457</v>
+      </c>
       <c r="C92" t="s">
         <v>361</v>
       </c>
@@ -3295,6 +3508,9 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>457</v>
+      </c>
       <c r="C93" t="s">
         <v>406</v>
       </c>
@@ -3306,6 +3522,9 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>457</v>
+      </c>
       <c r="C94" t="s">
         <v>407</v>
       </c>
@@ -3317,6 +3536,9 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>457</v>
+      </c>
       <c r="C95" t="s">
         <v>410</v>
       </c>
@@ -3328,6 +3550,9 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>457</v>
+      </c>
       <c r="C96" t="s">
         <v>412</v>
       </c>
@@ -3338,7 +3563,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>457</v>
+      </c>
       <c r="C97" t="s">
         <v>427</v>
       </c>
@@ -3349,8 +3577,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B98" s="6">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>457</v>
+      </c>
+      <c r="B98" s="5">
         <v>0.46458333333333335</v>
       </c>
       <c r="C98" t="s">
@@ -3363,8 +3594,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B99" s="6">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>457</v>
+      </c>
+      <c r="B99" s="5">
         <v>0.4680555555555555</v>
       </c>
       <c r="C99" t="s">
@@ -3377,8 +3611,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B100" s="6">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>457</v>
+      </c>
+      <c r="B100" s="5">
         <v>0.47222222222222227</v>
       </c>
       <c r="C100" t="s">
@@ -3391,8 +3628,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B101" s="6">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>457</v>
+      </c>
+      <c r="B101" s="5">
         <v>0.47222222222222227</v>
       </c>
       <c r="C101" t="s">
@@ -3405,8 +3645,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B102" s="6">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>442</v>
+      </c>
+      <c r="B102" s="5">
         <v>0.4770833333333333</v>
       </c>
       <c r="C102" t="s">
@@ -3419,8 +3662,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B103" s="6">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>442</v>
+      </c>
+      <c r="B103" s="5">
         <v>0.47500000000000003</v>
       </c>
       <c r="C103" t="s">
@@ -3433,13 +3679,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="6" t="s">
+        <v>442</v>
+      </c>
       <c r="B104" s="7">
         <v>0.47569444444444442</v>
       </c>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B105" s="6">
+      <c r="C104" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E104" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>442</v>
+      </c>
+      <c r="B105" s="5">
         <v>0.47638888888888892</v>
       </c>
       <c r="C105" t="s">
@@ -3452,12 +3710,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B106" s="6">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>442</v>
+      </c>
+      <c r="B106" s="5">
         <v>0.4770833333333333</v>
       </c>
       <c r="C106" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D106" t="s">
         <v>446</v>
@@ -3466,19 +3727,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>442</v>
+      </c>
       <c r="B107" s="7">
         <v>0.4770833333333333</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="C107" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D107" s="5" t="s">
+      <c r="D107" s="6" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B108" s="6">
+      <c r="E107" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>442</v>
+      </c>
+      <c r="B108" s="5">
         <v>0.47847222222222219</v>
       </c>
       <c r="C108" t="s">
@@ -3491,8 +3761,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B109" s="6">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>442</v>
+      </c>
+      <c r="B109" s="5">
         <v>0.47847222222222219</v>
       </c>
       <c r="C109" t="s">
@@ -3505,8 +3778,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B110" s="6">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>442</v>
+      </c>
+      <c r="B110" s="5">
         <v>0.47847222222222219</v>
       </c>
       <c r="C110" t="s">
@@ -3516,8 +3792,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B111" s="6">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>442</v>
+      </c>
+      <c r="B111" s="5">
         <v>0.47847222222222219</v>
       </c>
       <c r="C111" t="s">
@@ -3530,8 +3809,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B112" s="6">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>442</v>
+      </c>
+      <c r="B112" s="5">
         <v>0.48125000000000001</v>
       </c>
       <c r="C112" t="s">
@@ -3544,7 +3826,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>442</v>
+      </c>
       <c r="C113" t="s">
         <v>406</v>
       </c>
@@ -3555,7 +3840,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>442</v>
+      </c>
       <c r="C114" t="s">
         <v>276</v>
       </c>
@@ -3566,7 +3854,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>442</v>
+      </c>
       <c r="C115" t="s">
         <v>274</v>
       </c>
@@ -3577,7 +3868,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>442</v>
+      </c>
       <c r="C116" t="s">
         <v>416</v>
       </c>
@@ -3588,8 +3882,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B117" s="6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>442</v>
+      </c>
+      <c r="B117" s="5">
         <v>0.48819444444444443</v>
       </c>
       <c r="C117" t="s">
@@ -3602,8 +3899,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B118" s="6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>442</v>
+      </c>
+      <c r="B118" s="5">
         <v>0.48888888888888887</v>
       </c>
       <c r="C118" t="s">
@@ -3616,7 +3916,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>442</v>
+      </c>
       <c r="C119" t="s">
         <v>353</v>
       </c>
@@ -3627,7 +3930,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>442</v>
+      </c>
       <c r="C120" t="s">
         <v>336</v>
       </c>
@@ -3638,7 +3944,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>442</v>
+      </c>
       <c r="C121" t="s">
         <v>294</v>
       </c>
@@ -3649,8 +3958,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B122" s="6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>442</v>
+      </c>
+      <c r="B122" s="5">
         <v>0.49861111111111112</v>
       </c>
       <c r="C122" t="s">
@@ -3663,8 +3975,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B123" s="6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>442</v>
+      </c>
+      <c r="B123" s="5">
         <v>0.4993055555555555</v>
       </c>
       <c r="C123" t="s">
@@ -3677,8 +3992,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B124" s="6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>442</v>
+      </c>
+      <c r="B124" s="5">
         <v>0.5</v>
       </c>
       <c r="C124" t="s">
@@ -3691,8 +4009,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B125" s="6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>442</v>
+      </c>
+      <c r="B125" s="5">
         <v>0.50347222222222221</v>
       </c>
       <c r="C125" t="s">
@@ -3705,8 +4026,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B126" s="6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>442</v>
+      </c>
+      <c r="B126" s="5">
         <v>0.50486111111111109</v>
       </c>
       <c r="C126" t="s">
@@ -3716,11 +4040,14 @@
         <v>446</v>
       </c>
       <c r="E126">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B127" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>442</v>
+      </c>
+      <c r="B127" s="5">
         <v>0.50486111111111109</v>
       </c>
       <c r="C127" t="s">
@@ -3736,8 +4063,11 @@
         <v>458</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B128" s="6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>442</v>
+      </c>
+      <c r="B128" s="5">
         <v>0.50694444444444442</v>
       </c>
       <c r="C128" t="s">
@@ -3753,8 +4083,11 @@
         <v>458</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B129" s="6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>442</v>
+      </c>
+      <c r="B129" s="5">
         <v>0.5083333333333333</v>
       </c>
       <c r="C129" t="s">
@@ -3767,8 +4100,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B130" s="6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>442</v>
+      </c>
+      <c r="B130" s="5">
         <v>0.50902777777777775</v>
       </c>
       <c r="C130" t="s">
@@ -3781,8 +4117,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B131" s="6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>442</v>
+      </c>
+      <c r="B131" s="5">
         <v>0.50902777777777775</v>
       </c>
       <c r="C131" t="s">
@@ -3795,8 +4134,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B132" s="6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>442</v>
+      </c>
+      <c r="B132" s="5">
         <v>0.50972222222222219</v>
       </c>
       <c r="C132" t="s">
@@ -3809,8 +4151,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B133" s="6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>442</v>
+      </c>
+      <c r="B133" s="5">
         <v>0.51041666666666663</v>
       </c>
       <c r="C133" t="s">
@@ -3826,8 +4171,11 @@
         <v>458</v>
       </c>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B134" s="6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>442</v>
+      </c>
+      <c r="B134" s="5">
         <v>0.51041666666666663</v>
       </c>
       <c r="C134" t="s">
@@ -3843,8 +4191,11 @@
         <v>459</v>
       </c>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B135" s="6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>442</v>
+      </c>
+      <c r="B135" s="5">
         <v>0.52083333333333337</v>
       </c>
       <c r="C135" t="s">
@@ -3857,8 +4208,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B136" s="6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>442</v>
+      </c>
+      <c r="B136" s="5">
         <v>0.5229166666666667</v>
       </c>
       <c r="C136" t="s">
@@ -3871,8 +4225,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B137" s="6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>442</v>
+      </c>
+      <c r="B137" s="5">
         <v>0.5229166666666667</v>
       </c>
       <c r="C137" t="s">
@@ -3885,7 +4242,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>442</v>
+      </c>
       <c r="C138" t="s">
         <v>176</v>
       </c>
@@ -3896,8 +4256,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B139" s="6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>442</v>
+      </c>
+      <c r="B139" s="5">
         <v>0.5229166666666667</v>
       </c>
       <c r="C139" t="s">
@@ -3910,23 +4273,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="6" t="s">
+        <v>442</v>
+      </c>
       <c r="B140" s="7"/>
-      <c r="C140" s="5" t="s">
+      <c r="C140" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="D140" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="E140" s="5">
-        <v>1</v>
-      </c>
-      <c r="F140" s="5" t="s">
+      <c r="D140" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E140" s="6">
+        <v>1</v>
+      </c>
+      <c r="F140" s="6" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B141" s="6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>442</v>
+      </c>
+      <c r="B141" s="5">
         <v>0.52500000000000002</v>
       </c>
       <c r="C141" t="s">
@@ -3939,8 +4308,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B142" s="6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>442</v>
+      </c>
+      <c r="B142" s="5">
         <v>0.52500000000000002</v>
       </c>
       <c r="C142" t="s">
@@ -3953,8 +4325,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B143" s="6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>442</v>
+      </c>
+      <c r="B143" s="5">
         <v>0.52569444444444446</v>
       </c>
       <c r="C143" t="s">
@@ -3967,8 +4342,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B144" s="6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>442</v>
+      </c>
+      <c r="B144" s="5">
         <v>0.52708333333333335</v>
       </c>
       <c r="C144" t="s">
@@ -3981,8 +4359,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B145" s="6">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>442</v>
+      </c>
+      <c r="B145" s="5">
         <v>0.54236111111111118</v>
       </c>
       <c r="C145" t="s">
@@ -3995,8 +4376,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B146" s="6">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>442</v>
+      </c>
+      <c r="B146" s="5">
         <v>0.54375000000000007</v>
       </c>
       <c r="C146" t="s">
@@ -4009,8 +4393,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B147" s="6">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>442</v>
+      </c>
+      <c r="B147" s="5">
         <v>0.54375000000000007</v>
       </c>
       <c r="C147" t="s">
@@ -4023,8 +4410,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B148" s="6">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>467</v>
+      </c>
+      <c r="B148" s="5">
         <v>0.55138888888888882</v>
       </c>
       <c r="C148" t="s">
@@ -4037,8 +4427,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B149" s="6">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>467</v>
+      </c>
+      <c r="B149" s="5">
         <v>0.55347222222222225</v>
       </c>
       <c r="C149" t="s">
@@ -4051,8 +4444,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B150" s="6">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>467</v>
+      </c>
+      <c r="B150" s="5">
         <v>0.5541666666666667</v>
       </c>
       <c r="C150" t="s">
@@ -4065,8 +4461,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B151" s="6">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>467</v>
+      </c>
+      <c r="B151" s="5">
         <v>0.55486111111111114</v>
       </c>
       <c r="C151" t="s">
@@ -4079,8 +4478,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B152" s="6">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>467</v>
+      </c>
+      <c r="B152" s="5">
         <v>0.55694444444444446</v>
       </c>
       <c r="C152" t="s">
@@ -4093,8 +4495,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B153" s="6">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>467</v>
+      </c>
+      <c r="B153" s="5">
         <v>0.55694444444444446</v>
       </c>
       <c r="C153" t="s">
@@ -4107,8 +4512,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B154" s="6">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>467</v>
+      </c>
+      <c r="B154" s="5">
         <v>0.55694444444444446</v>
       </c>
       <c r="C154" t="s">
@@ -4121,8 +4529,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B155" s="6">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>467</v>
+      </c>
+      <c r="B155" s="5">
         <v>0.55763888888888891</v>
       </c>
       <c r="C155" t="s">
@@ -4135,8 +4546,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B156" s="6">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>467</v>
+      </c>
+      <c r="B156" s="5">
         <v>0.55972222222222223</v>
       </c>
       <c r="C156" t="s">
@@ -4149,8 +4563,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B157" s="6">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>467</v>
+      </c>
+      <c r="B157" s="5">
         <v>0.56874999999999998</v>
       </c>
       <c r="C157" t="s">
@@ -4163,8 +4580,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B158" s="6">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>440</v>
+      </c>
+      <c r="B158" s="5">
         <v>0.57430555555555551</v>
       </c>
       <c r="C158" t="s">
@@ -4177,8 +4597,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B159" s="6">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>440</v>
+      </c>
+      <c r="B159" s="5">
         <v>0.57708333333333328</v>
       </c>
       <c r="C159" t="s">
@@ -4191,7 +4614,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>440</v>
+      </c>
       <c r="C160" t="s">
         <v>393</v>
       </c>
@@ -4202,7 +4628,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>440</v>
+      </c>
       <c r="C161" t="s">
         <v>244</v>
       </c>
@@ -4216,8 +4645,11 @@
         <v>462</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B162" s="6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>440</v>
+      </c>
+      <c r="B162" s="5">
         <v>0.57986111111111105</v>
       </c>
       <c r="C162" t="s">
@@ -4230,8 +4662,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B163" s="6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>440</v>
+      </c>
+      <c r="B163" s="5">
         <v>0.58124999999999993</v>
       </c>
       <c r="C163" t="s">
@@ -4244,16 +4679,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="6" t="s">
+        <v>440</v>
+      </c>
       <c r="B164" s="7">
         <v>0.58194444444444449</v>
       </c>
-      <c r="C164" s="5" t="s">
+      <c r="C164" s="6" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B165" s="6">
+      <c r="E164" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>440</v>
+      </c>
+      <c r="B165" s="5">
         <v>0.58333333333333337</v>
       </c>
       <c r="C165" t="s">
@@ -4266,8 +4710,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B166" s="6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>440</v>
+      </c>
+      <c r="B166" s="5">
         <v>0.58402777777777781</v>
       </c>
       <c r="C166" t="s">
@@ -4280,7 +4727,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>440</v>
+      </c>
       <c r="C167" t="s">
         <v>221</v>
       </c>
@@ -4288,7 +4738,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>440</v>
+      </c>
       <c r="C168" t="s">
         <v>269</v>
       </c>
@@ -4296,7 +4749,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>440</v>
+      </c>
       <c r="C169" t="s">
         <v>276</v>
       </c>
@@ -4304,16 +4760,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="6" t="s">
+        <v>440</v>
+      </c>
       <c r="B170" s="7"/>
-      <c r="C170" s="5" t="s">
+      <c r="C170" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="E170" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E170" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>440</v>
+      </c>
       <c r="C171" t="s">
         <v>316</v>
       </c>
@@ -4321,7 +4783,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>440</v>
+      </c>
       <c r="C172" t="s">
         <v>353</v>
       </c>
@@ -4329,7 +4794,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>440</v>
+      </c>
       <c r="C173" t="s">
         <v>401</v>
       </c>
@@ -4337,7 +4805,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>440</v>
+      </c>
       <c r="C174" t="s">
         <v>409</v>
       </c>
@@ -4345,7 +4816,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>440</v>
+      </c>
       <c r="C175" t="s">
         <v>415</v>
       </c>
@@ -4353,7 +4827,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>440</v>
+      </c>
       <c r="C176" t="s">
         <v>417</v>
       </c>
@@ -4361,8 +4838,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B177" s="6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>468</v>
+      </c>
+      <c r="B177" s="5">
         <v>0.62986111111111109</v>
       </c>
       <c r="C177" t="s">
@@ -4375,7 +4855,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>468</v>
+      </c>
       <c r="C178" t="s">
         <v>348</v>
       </c>
@@ -4383,7 +4866,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>468</v>
+      </c>
       <c r="C179" t="s">
         <v>173</v>
       </c>
@@ -4391,8 +4877,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B180" s="6">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>468</v>
+      </c>
+      <c r="B180" s="5">
         <v>0.63194444444444442</v>
       </c>
       <c r="C180" t="s">
@@ -4402,8 +4891,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B181" s="6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>468</v>
+      </c>
+      <c r="B181" s="5">
         <v>0.63194444444444442</v>
       </c>
       <c r="C181" t="s">
@@ -4413,8 +4905,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B182" s="6">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>468</v>
+      </c>
+      <c r="B182" s="5">
         <v>0.63194444444444442</v>
       </c>
       <c r="C182" t="s">
@@ -4424,8 +4919,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B183" s="6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>468</v>
+      </c>
+      <c r="B183" s="5">
         <v>0.63402777777777775</v>
       </c>
       <c r="C183" t="s">
@@ -4438,8 +4936,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B184" s="6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>468</v>
+      </c>
+      <c r="B184" s="5">
         <v>0.63472222222222219</v>
       </c>
       <c r="C184" t="s">
@@ -4449,8 +4950,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B185" s="6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>468</v>
+      </c>
+      <c r="B185" s="5">
         <v>0.63541666666666663</v>
       </c>
       <c r="C185" t="s">
@@ -4466,7 +4970,10 @@
         <v>453</v>
       </c>
     </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>468</v>
+      </c>
       <c r="C186" t="s">
         <v>37</v>
       </c>
@@ -4477,7 +4984,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>468</v>
+      </c>
       <c r="C187" t="s">
         <v>422</v>
       </c>
@@ -4485,7 +4995,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>468</v>
+      </c>
       <c r="C188" t="s">
         <v>104</v>
       </c>
@@ -4493,7 +5006,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>468</v>
+      </c>
       <c r="C189" t="s">
         <v>174</v>
       </c>
@@ -4501,16 +5017,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="6" t="s">
+        <v>468</v>
+      </c>
       <c r="B190" s="7">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C190" s="5" t="s">
+      <c r="C190" s="6" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B191" s="6">
+      <c r="E190" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>435</v>
+      </c>
+      <c r="B191" s="5">
         <v>0.64097222222222217</v>
       </c>
       <c r="C191" t="s">
@@ -4523,8 +5048,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B192" s="6">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>435</v>
+      </c>
+      <c r="B192" s="5">
         <v>0.64097222222222217</v>
       </c>
       <c r="C192" t="s">
@@ -4537,8 +5065,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B193" s="6">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>435</v>
+      </c>
+      <c r="B193" s="5">
         <v>0.64166666666666672</v>
       </c>
       <c r="C193" t="s">
@@ -4551,8 +5082,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B194" s="6">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>435</v>
+      </c>
+      <c r="B194" s="5">
         <v>0.64236111111111105</v>
       </c>
       <c r="C194" t="s">
@@ -4565,8 +5099,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B195" s="6">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>435</v>
+      </c>
+      <c r="B195" s="5">
         <v>0.6430555555555556</v>
       </c>
       <c r="C195" t="s">
@@ -4579,8 +5116,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B196" s="6">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>435</v>
+      </c>
+      <c r="B196" s="5">
         <v>0.64374999999999993</v>
       </c>
       <c r="C196" t="s">
@@ -4593,8 +5133,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B197" s="6">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>435</v>
+      </c>
+      <c r="B197" s="5">
         <v>0.64374999999999993</v>
       </c>
       <c r="C197" t="s">
@@ -4607,8 +5150,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B198" s="6">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>435</v>
+      </c>
+      <c r="B198" s="5">
         <v>0.64444444444444449</v>
       </c>
       <c r="C198" t="s">
@@ -4621,22 +5167,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="6" t="s">
+        <v>435</v>
+      </c>
       <c r="B199" s="7">
         <v>0.64444444444444449</v>
       </c>
-      <c r="C199" s="5" t="s">
+      <c r="C199" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D199" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="E199" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B200" s="6">
+      <c r="D199" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E199" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>435</v>
+      </c>
+      <c r="B200" s="5">
         <v>0.64513888888888882</v>
       </c>
       <c r="C200" t="s">
@@ -4649,8 +5201,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B201" s="6">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>435</v>
+      </c>
+      <c r="B201" s="5">
         <v>0.64513888888888882</v>
       </c>
       <c r="C201" t="s">
@@ -4663,8 +5218,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B202" s="6">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>435</v>
+      </c>
+      <c r="B202" s="5">
         <v>0.64513888888888882</v>
       </c>
       <c r="C202" t="s">
@@ -4677,8 +5235,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B203" s="6">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>435</v>
+      </c>
+      <c r="B203" s="5">
         <v>0.64583333333333337</v>
       </c>
       <c r="C203" t="s">
@@ -4691,8 +5252,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B204" s="6">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>435</v>
+      </c>
+      <c r="B204" s="5">
         <v>0.64722222222222225</v>
       </c>
       <c r="C204" t="s">
@@ -4705,8 +5269,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B205" s="6">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>436</v>
+      </c>
+      <c r="B205" s="5">
         <v>0.6479166666666667</v>
       </c>
       <c r="C205" t="s">
@@ -4719,8 +5286,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B206" s="6">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>436</v>
+      </c>
+      <c r="B206" s="5">
         <v>0.64930555555555558</v>
       </c>
       <c r="C206" t="s">
@@ -4733,8 +5303,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B207" s="6">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>436</v>
+      </c>
+      <c r="B207" s="5">
         <v>0.65069444444444446</v>
       </c>
       <c r="C207" t="s">
@@ -4747,8 +5320,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B208" s="6">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>436</v>
+      </c>
+      <c r="B208" s="5">
         <v>0.65069444444444446</v>
       </c>
       <c r="C208" t="s">
@@ -4761,8 +5337,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B209" s="6">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>436</v>
+      </c>
+      <c r="B209" s="5">
         <v>0.65208333333333335</v>
       </c>
       <c r="C209" t="s">
@@ -4775,8 +5354,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B210" s="6">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>436</v>
+      </c>
+      <c r="B210" s="5">
         <v>0.65208333333333335</v>
       </c>
       <c r="C210" t="s">
@@ -4789,8 +5371,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B211" s="6">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>436</v>
+      </c>
+      <c r="B211" s="5">
         <v>0.65277777777777779</v>
       </c>
       <c r="C211" t="s">
@@ -4803,8 +5388,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B212" s="6">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>436</v>
+      </c>
+      <c r="B212" s="5">
         <v>0.65277777777777779</v>
       </c>
       <c r="C212" t="s">
@@ -4817,8 +5405,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B213" s="6">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>436</v>
+      </c>
+      <c r="B213" s="5">
         <v>0.65416666666666667</v>
       </c>
       <c r="C213" t="s">
@@ -4834,8 +5425,11 @@
         <v>454</v>
       </c>
     </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B214" s="6">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>436</v>
+      </c>
+      <c r="B214" s="5">
         <v>0.65625</v>
       </c>
       <c r="C214" t="s">
@@ -4848,8 +5442,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B215" s="6">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>469</v>
+      </c>
+      <c r="B215" s="5">
         <v>0.66111111111111109</v>
       </c>
       <c r="C215" t="s">
@@ -4862,8 +5459,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B216" s="6">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>469</v>
+      </c>
+      <c r="B216" s="5">
         <v>0.66249999999999998</v>
       </c>
       <c r="C216" t="s">
@@ -4876,8 +5476,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B217" s="6">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>469</v>
+      </c>
+      <c r="B217" s="5">
         <v>0.66597222222222219</v>
       </c>
       <c r="C217" t="s">
@@ -4890,8 +5493,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B218" s="6">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>469</v>
+      </c>
+      <c r="B218" s="5">
         <v>0.66597222222222219</v>
       </c>
       <c r="C218" t="s">
@@ -4904,8 +5510,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B219" s="6">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>469</v>
+      </c>
+      <c r="B219" s="5">
         <v>0.66666666666666663</v>
       </c>
       <c r="C219" t="s">
@@ -4918,8 +5527,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B220" s="6">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>469</v>
+      </c>
+      <c r="B220" s="5">
         <v>0.66666666666666663</v>
       </c>
       <c r="C220" t="s">
@@ -4932,8 +5544,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B221" s="6">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>469</v>
+      </c>
+      <c r="B221" s="5">
         <v>0.66805555555555562</v>
       </c>
       <c r="C221" t="s">
@@ -4946,8 +5561,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B222" s="6">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>469</v>
+      </c>
+      <c r="B222" s="5">
         <v>0.66805555555555562</v>
       </c>
       <c r="C222" t="s">
@@ -4967,7 +5585,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{032B9681-8078-114D-82A1-72B19DA841C3}">
           <x14:formula1>
-            <xm:f>validación!$A$2:$A$18</xm:f>
+            <xm:f>validación!$A$2:$A$25</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A1048576</xm:sqref>
         </x14:dataValidation>
@@ -4993,8 +5611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56384002-26E4-974C-A569-A4D9FCD70CC0}">
   <dimension ref="A1:C428"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B429" sqref="B429"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5160,36 +5778,57 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>463</v>
+      </c>
       <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>464</v>
+      </c>
       <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>465</v>
+      </c>
       <c r="B21" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>466</v>
+      </c>
       <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>467</v>
+      </c>
       <c r="B23" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>468</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>469</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>